<commit_message>
Added Power BI Template
</commit_message>
<xml_diff>
--- a/personal-spendings.xlsx
+++ b/personal-spendings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Repos\Medium\dynamic-pivot-in-powerbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C1229-C1C7-4DDD-85B2-5C4196776446}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8E36FE-0A4E-4E65-A9BC-BFB5DEDEBFAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28702" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{D9C87DA8-FAB7-4F4F-A026-A2C9D20D96C5}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +110,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,11 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,11 +452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8C6A32-DA70-46CD-BB0F-C300CC61F071}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C135" sqref="C135"/>
+      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2753,13 +2744,6 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="3"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{B66146A0-C9CF-4286-8803-7C8C58342347}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>